<commit_message>
[#3] When cell contains a formula, value is always returned.
</commit_message>
<xml_diff>
--- a/cdc-office-ss-excel/src/test/resources/file1.xlsx
+++ b/cdc-office-ss-excel/src/test/resources/file1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="file1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
   </si>
   <si>
     <t xml:space="preserve">Hello</t>
@@ -139,35 +142,35 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="12.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.33673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.77040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.73469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.16326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.27040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,22 +189,29 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">A2+C2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -209,16 +219,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">A3+C3</f>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,22 +240,26 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
+      <c r="F4" s="0" t="n">
+        <f aca="false">A4+C4</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>